<commit_message>
Sprint 6 Izaquiel burndown
</commit_message>
<xml_diff>
--- a/Sprint 6/Sprint_6 Burndown-Backlog.xlsx
+++ b/Sprint 6/Sprint_6 Burndown-Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaquiel\Desktop\PDS\Sprint 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -127,35 +127,7 @@
     <t>Módulo Agendamento</t>
   </si>
   <si>
-    <t>Terça
-11/10/2016</t>
-  </si>
-  <si>
     <t>Reajuste de código</t>
-  </si>
-  <si>
-    <t>Quarta
-12/10/2016</t>
-  </si>
-  <si>
-    <t>Quinta
-13/10/2016</t>
-  </si>
-  <si>
-    <t>Sexta
-14/10/2016</t>
-  </si>
-  <si>
-    <t>Sábado
-15/10/2016</t>
-  </si>
-  <si>
-    <t>Domingo
-16/10/2016</t>
-  </si>
-  <si>
-    <t>Segunda
-17/10/2016</t>
   </si>
   <si>
     <t>Terça
@@ -208,6 +180,34 @@
   </si>
   <si>
     <t>Estudo da funcionalidade</t>
+  </si>
+  <si>
+    <t>Quarta
+19/10/2016</t>
+  </si>
+  <si>
+    <t>Quinta
+20/10/2016</t>
+  </si>
+  <si>
+    <t>Sexta
+21/10/2016</t>
+  </si>
+  <si>
+    <t>Sábado
+22/10/2016</t>
+  </si>
+  <si>
+    <t>Domingo
+23/10/2016</t>
+  </si>
+  <si>
+    <t>Segunda
+24/10/2016</t>
+  </si>
+  <si>
+    <t>Terça
+25/10/2016</t>
   </si>
 </sst>
 </file>
@@ -597,13 +597,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,6 +626,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -676,9 +679,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2599,35 +2599,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2732,35 +2732,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2787,16 +2787,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-14.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-25.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-25.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-35.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2824,11 +2824,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="196585208"/>
-        <c:axId val="195836920"/>
+        <c:axId val="385501200"/>
+        <c:axId val="385506296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196585208"/>
+        <c:axId val="385501200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2909,7 +2909,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195836920"/>
+        <c:crossAx val="385506296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2917,7 +2917,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195836920"/>
+        <c:axId val="385506296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,6 +2968,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2999,7 +3000,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196585208"/>
+        <c:crossAx val="385501200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3012,6 +3013,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3108,35 +3110,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3241,35 +3243,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3296,16 +3298,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-7.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-12.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3333,11 +3335,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="195875216"/>
-        <c:axId val="197134248"/>
+        <c:axId val="385507472"/>
+        <c:axId val="385505512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195875216"/>
+        <c:axId val="385507472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3379,6 +3381,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3410,7 +3413,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197134248"/>
+        <c:crossAx val="385505512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3418,7 +3421,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197134248"/>
+        <c:axId val="385505512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3469,6 +3472,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3500,7 +3504,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195875216"/>
+        <c:crossAx val="385507472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3513,6 +3517,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3609,35 +3614,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3742,35 +3747,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3797,16 +3802,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-9.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-11.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3834,11 +3839,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="196015240"/>
-        <c:axId val="195859376"/>
+        <c:axId val="385507864"/>
+        <c:axId val="385501984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196015240"/>
+        <c:axId val="385507864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3880,6 +3885,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3911,7 +3917,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195859376"/>
+        <c:crossAx val="385501984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3919,7 +3925,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195859376"/>
+        <c:axId val="385501984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,6 +3976,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4001,7 +4008,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196015240"/>
+        <c:crossAx val="385507864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4014,6 +4021,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4110,35 +4118,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4243,35 +4251,35 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Terça
-11/10/2016</c:v>
+18/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Quarta
-12/10/2016</c:v>
+19/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Quinta
-13/10/2016</c:v>
+20/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sexta
-14/10/2016</c:v>
+21/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sábado
-15/10/2016</c:v>
+22/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Domingo
-16/10/2016</c:v>
+23/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Segunda
-17/10/2016</c:v>
+24/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Terça
-18/10/2016</c:v>
+25/10/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4298,16 +4306,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-8.6999999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-8.6999999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-11.899999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4335,11 +4343,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="196767208"/>
-        <c:axId val="195864080"/>
+        <c:axId val="385501592"/>
+        <c:axId val="385504728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196767208"/>
+        <c:axId val="385501592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4381,6 +4389,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4412,7 +4421,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195864080"/>
+        <c:crossAx val="385504728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4420,7 +4429,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195864080"/>
+        <c:axId val="385504728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4471,6 +4480,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4502,7 +4512,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196767208"/>
+        <c:crossAx val="385501592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4515,6 +4525,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4983,8 +4994,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048575"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView windowProtection="1" showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5117,11 +5128,11 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>43</v>
+      <c r="A4" s="36" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -5135,7 +5146,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="3"/>
@@ -5159,9 +5170,9 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -5193,7 +5204,7 @@
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="38"/>
       <c r="B6" s="24" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5201,7 +5212,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="40"/>
       <c r="H6" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I6" s="22"/>
       <c r="J6" s="3"/>
@@ -5226,10 +5237,10 @@
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="31"/>
@@ -5237,7 +5248,7 @@
       <c r="F7" s="31"/>
       <c r="G7" s="40"/>
       <c r="H7" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5259,9 +5270,9 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="24" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="20"/>
@@ -5269,7 +5280,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="40"/>
       <c r="H8" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -5291,9 +5302,9 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="20"/>
@@ -5301,7 +5312,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="40"/>
       <c r="H9" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I9" s="6"/>
       <c r="K9" s="4"/>
@@ -5324,9 +5335,9 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="26" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -5334,7 +5345,7 @@
       <c r="F10" s="20"/>
       <c r="G10" s="40"/>
       <c r="H10" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I10" s="6"/>
       <c r="K10" s="4"/>
@@ -5358,10 +5369,10 @@
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -5390,9 +5401,9 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="26" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -5400,7 +5411,7 @@
       <c r="F12" s="20"/>
       <c r="G12" s="40"/>
       <c r="H12" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I12" s="6"/>
       <c r="K12" s="4"/>
@@ -5424,18 +5435,20 @@
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="20"/>
+        <v>49</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
       <c r="F13" s="20"/>
       <c r="G13" s="40"/>
       <c r="H13" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I13" s="6"/>
       <c r="K13" s="4"/>
@@ -5458,17 +5471,19 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="20"/>
+        <v>48</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="44"/>
       <c r="F14" s="20"/>
       <c r="G14" s="41"/>
       <c r="H14" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I14" s="6"/>
       <c r="K14" s="4"/>
@@ -5749,6 +5764,13 @@
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A4:A6"/>
@@ -5756,13 +5778,6 @@
     <mergeCell ref="E4:E14"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I6">
     <cfRule type="expression" dxfId="125" priority="2">
@@ -5786,7 +5801,7 @@
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5807,20 +5822,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -5879,40 +5894,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47">
+      <c r="A3" s="48">
         <v>8</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="48" t="s">
+      <c r="C3" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="49" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -5924,18 +5939,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -6026,27 +6041,27 @@
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>-14.2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>-25.7</v>
+        <v>0</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>-25.7</v>
+        <v>0</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>-35.9</v>
+        <v>0</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>-101.5</v>
+        <v>0</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>-12.6875</v>
+        <v>0</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -6084,18 +6099,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -6130,11 +6145,11 @@
       </c>
       <c r="G9" s="16">
         <f t="shared" si="3"/>
-        <v>14.2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="16">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="3"/>
@@ -6142,15 +6157,15 @@
       </c>
       <c r="J9" s="16">
         <f t="shared" si="3"/>
-        <v>10.199999999999999</v>
+        <v>0</v>
       </c>
       <c r="K9" s="16">
         <f t="shared" si="3"/>
-        <v>35.9</v>
+        <v>0</v>
       </c>
       <c r="L9" s="16">
         <f>K9/A$3</f>
-        <v>4.4874999999999998</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -6183,25 +6198,25 @@
         <v>0</v>
       </c>
       <c r="G10" s="13">
-        <v>4.25</v>
+        <v>0</v>
       </c>
       <c r="H10" s="13">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I10" s="13">
         <f>Diogo!I9</f>
         <v>0</v>
       </c>
       <c r="J10" s="13">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="K10" s="13">
         <f>SUM(C10:J10)</f>
-        <v>12.25</v>
+        <v>0</v>
       </c>
       <c r="L10" s="13">
         <f>K10/A$3</f>
-        <v>1.53125</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -6233,24 +6248,24 @@
         <v>0</v>
       </c>
       <c r="G11" s="13">
-        <v>5.75</v>
+        <v>0</v>
       </c>
       <c r="H11" s="13">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I11" s="13">
         <v>0</v>
       </c>
       <c r="J11" s="13">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K11" s="13">
         <f>SUM(C11:J11)</f>
-        <v>11.75</v>
+        <v>0</v>
       </c>
       <c r="L11" s="13">
         <f>K11/A$3</f>
-        <v>1.46875</v>
+        <v>0</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -6283,24 +6298,24 @@
         <v>0</v>
       </c>
       <c r="G12" s="13">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="13">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="I12" s="13">
         <v>0</v>
       </c>
       <c r="J12" s="13">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="13">
         <f>SUM(C12:J12)</f>
-        <v>11.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="L12" s="13">
         <f>K12/A$3</f>
-        <v>1.4874999999999998</v>
+        <v>0</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -6838,7 +6853,7 @@
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6852,20 +6867,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -6924,40 +6939,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47">
+      <c r="A3" s="48">
         <v>8</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="48" t="s">
+      <c r="C3" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="49" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -6969,18 +6984,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -7071,27 +7086,27 @@
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>-4.25</v>
+        <v>0</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>-7.75</v>
+        <v>0</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>-7.75</v>
+        <v>0</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>-12.25</v>
+        <v>0</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>-32</v>
+        <v>0</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -7129,18 +7144,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -7175,11 +7190,11 @@
       </c>
       <c r="G9" s="16">
         <f t="shared" si="3"/>
-        <v>4.25</v>
+        <v>0</v>
       </c>
       <c r="H9" s="16">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="3"/>
@@ -7187,15 +7202,15 @@
       </c>
       <c r="J9" s="16">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="K9" s="16">
         <f t="shared" si="3"/>
-        <v>12.25</v>
+        <v>0</v>
       </c>
       <c r="L9" s="16">
         <f t="shared" si="3"/>
-        <v>1.53125</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -7206,10 +7221,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="58"/>
+      <c r="A10" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="59"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -7223,10 +7238,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="13">
-        <v>4.25</v>
+        <v>0</v>
       </c>
       <c r="H10" s="13">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I10" s="13">
         <v>0</v>
@@ -7236,25 +7251,25 @@
       </c>
       <c r="K10" s="13">
         <f>SUM(C10:J10)</f>
-        <v>7.75</v>
+        <v>0</v>
       </c>
       <c r="L10" s="13">
         <f>K10/A$3</f>
-        <v>0.96875</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="61"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -7277,29 +7292,29 @@
         <v>0</v>
       </c>
       <c r="J11" s="13">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="K11" s="13">
         <f>SUM(C11:J11)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="L11" s="13">
         <f>K11/A$3</f>
-        <v>0.5625</v>
+        <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="55"/>
+      <c r="A12" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="56"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -7333,8 +7348,8 @@
         <v>0</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
@@ -7342,8 +7357,8 @@
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -7354,14 +7369,6 @@
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -7376,6 +7383,14 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:L96 N10:O12 B13:C13">
     <cfRule type="expression" dxfId="24" priority="2">
@@ -7415,7 +7430,7 @@
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7429,20 +7444,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -7501,40 +7516,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47">
+      <c r="A3" s="48">
         <v>8</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="48" t="s">
+      <c r="C3" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="49" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -7546,18 +7561,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -7648,27 +7663,27 @@
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>-5.75</v>
+        <v>0</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>-9.25</v>
+        <v>0</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>-9.25</v>
+        <v>0</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>-11.75</v>
+        <v>0</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>-36</v>
+        <v>0</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>-4.5</v>
+        <v>0</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -7706,18 +7721,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -7752,11 +7767,11 @@
       </c>
       <c r="G9" s="16">
         <f t="shared" si="3"/>
-        <v>5.75</v>
+        <v>0</v>
       </c>
       <c r="H9" s="16">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="3"/>
@@ -7764,15 +7779,15 @@
       </c>
       <c r="J9" s="16">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K9" s="16">
         <f t="shared" si="3"/>
-        <v>11.75</v>
+        <v>0</v>
       </c>
       <c r="L9" s="16">
         <f t="shared" si="3"/>
-        <v>1.46875</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -7783,10 +7798,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="58"/>
+      <c r="A10" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="59"/>
       <c r="C10" s="21">
         <v>0</v>
       </c>
@@ -7828,10 +7843,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="61"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="21">
         <v>0</v>
       </c>
@@ -7845,10 +7860,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="21">
-        <v>5.75</v>
+        <v>0</v>
       </c>
       <c r="H11" s="21">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I11" s="21">
         <v>0</v>
@@ -7858,11 +7873,11 @@
       </c>
       <c r="K11" s="21">
         <f>SUM(C11:J11)</f>
-        <v>9.25</v>
+        <v>0</v>
       </c>
       <c r="L11" s="21">
         <f>K11/A$3</f>
-        <v>1.15625</v>
+        <v>0</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -7873,10 +7888,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="55"/>
+      <c r="A12" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="56"/>
       <c r="C12" s="21">
         <v>0</v>
       </c>
@@ -7899,15 +7914,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="21">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K12" s="21">
         <f>SUM(C12:J12)</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="L12" s="21">
         <f>K12/A$3</f>
-        <v>0.3125</v>
+        <v>0</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -7932,6 +7947,8 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -7948,8 +7965,6 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:L96 K10:L12">
     <cfRule type="expression" dxfId="19" priority="14">
@@ -8010,9 +8025,9 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8026,20 +8041,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -8098,40 +8113,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47">
+      <c r="A3" s="48">
         <v>8</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="48" t="s">
+      <c r="C3" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="49" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -8143,18 +8158,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -8245,27 +8260,27 @@
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>-4.2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>-8.6999999999999993</v>
+        <v>0</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>-8.6999999999999993</v>
+        <v>0</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>-11.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>-33.5</v>
+        <v>0</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>-4.1875</v>
+        <v>0</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -8303,18 +8318,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -8349,11 +8364,11 @@
       </c>
       <c r="G9" s="16">
         <f t="shared" si="3"/>
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="16">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="3"/>
@@ -8361,15 +8376,15 @@
       </c>
       <c r="J9" s="16">
         <f t="shared" si="3"/>
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="K9" s="16">
         <f t="shared" si="3"/>
-        <v>11.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="L9" s="16">
         <f t="shared" si="3"/>
-        <v>1.4874999999999998</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -8380,10 +8395,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="58"/>
+      <c r="A10" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="59"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -8425,10 +8440,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="61"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -8442,10 +8457,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="13">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="H11" s="13">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="I11" s="13">
         <v>0</v>
@@ -8455,11 +8470,11 @@
       </c>
       <c r="K11" s="13">
         <f>SUM(C11:J11)</f>
-        <v>8.6999999999999993</v>
+        <v>0</v>
       </c>
       <c r="L11" s="13">
         <f>K11/A$3</f>
-        <v>1.0874999999999999</v>
+        <v>0</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -8470,10 +8485,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="55"/>
+      <c r="A12" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="56"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -8496,15 +8511,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="13">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="13">
         <f>SUM(C12:J12)</f>
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="L12" s="13">
         <f>K12/A$3</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -8529,6 +8544,8 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -8545,8 +8562,6 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:L96 K10:L12">
     <cfRule type="expression" dxfId="9" priority="12">

</xml_diff>